<commit_message>
adds dotenv to requirements for real
</commit_message>
<xml_diff>
--- a/excel_files/accurate_dol_geocoded.xlsx
+++ b/excel_files/accurate_dol_geocoded.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexpiazza/Desktop/for_db/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F391060C-A7CE-3648-8C33-83A2B5E31CBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747BE93D-BF43-FF4C-99D4-C3E7504C08E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1605,8 +1605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:EU8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DC1" workbookViewId="0">
-      <selection activeCell="DN8" sqref="DN8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1614,6 +1614,7 @@
     <col min="1" max="1" width="33.83203125" customWidth="1"/>
     <col min="7" max="7" width="20.5" customWidth="1"/>
     <col min="9" max="9" width="36.1640625" customWidth="1"/>
+    <col min="10" max="10" width="34.5" customWidth="1"/>
     <col min="112" max="112" width="29.1640625" customWidth="1"/>
     <col min="118" max="118" width="29.33203125" customWidth="1"/>
     <col min="119" max="119" width="23.6640625" customWidth="1"/>

</xml_diff>

<commit_message>
updates tests and dol scripts
</commit_message>
<xml_diff>
--- a/excel_files/accurate_dol_geocoded.xlsx
+++ b/excel_files/accurate_dol_geocoded.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexpiazza/Desktop/for_db/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747BE93D-BF43-FF4C-99D4-C3E7504C08E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FEAFC36-E29E-9E4C-B2C0-B2E1C4D92057}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -292,9 +292,6 @@
     <t>790A_addendum_a_attached</t>
   </si>
   <si>
-    <t>FREQUENCY_OF_PAY</t>
-  </si>
-  <si>
     <t>OTHER_FREQUENCY_OF_PAY</t>
   </si>
   <si>
@@ -1185,6 +1182,9 @@
   </si>
   <si>
     <t>H-300-20125-5389134</t>
+  </si>
+  <si>
+    <t>Additional Wage Information</t>
   </si>
 </sst>
 </file>
@@ -1605,8 +1605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:EU8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="BZ1" workbookViewId="0">
+      <selection activeCell="CN1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1895,195 +1895,195 @@
         <v>89</v>
       </c>
       <c r="CM1" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="CN1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="CN1" s="1" t="s">
+      <c r="CO1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="CO1" s="1" t="s">
+      <c r="CP1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="CP1" s="1" t="s">
+      <c r="CQ1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="CQ1" s="1" t="s">
+      <c r="CR1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="CR1" s="1" t="s">
+      <c r="CS1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="CS1" s="1" t="s">
+      <c r="CT1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="CT1" s="1" t="s">
+      <c r="CU1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="CU1" s="1" t="s">
+      <c r="CV1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="CV1" s="1" t="s">
+      <c r="CW1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="CW1" s="1" t="s">
+      <c r="CX1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="CX1" s="1" t="s">
+      <c r="CY1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="CY1" s="1" t="s">
+      <c r="CZ1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="CZ1" s="1" t="s">
+      <c r="DA1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="DA1" s="1" t="s">
+      <c r="DB1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="DB1" s="1" t="s">
+      <c r="DC1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="DC1" s="1" t="s">
+      <c r="DD1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="DD1" s="1" t="s">
+      <c r="DE1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="DE1" s="1" t="s">
+      <c r="DF1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="DF1" s="1" t="s">
+      <c r="DG1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="DG1" s="1" t="s">
+      <c r="DH1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="DH1" s="1" t="s">
+      <c r="DI1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="DI1" s="1" t="s">
+      <c r="DJ1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="DJ1" s="1" t="s">
+      <c r="DK1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="DK1" s="1" t="s">
+      <c r="DL1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="DL1" s="1" t="s">
+      <c r="DM1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="DM1" s="1" t="s">
+      <c r="DN1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="DN1" s="1" t="s">
+      <c r="DO1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="DO1" s="1" t="s">
+      <c r="DP1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="DP1" s="1" t="s">
+      <c r="DQ1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="DQ1" s="1" t="s">
+      <c r="DR1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="DR1" s="1" t="s">
+      <c r="DS1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="DS1" s="1" t="s">
+      <c r="DT1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="DT1" s="1" t="s">
+      <c r="DU1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="DU1" s="1" t="s">
+      <c r="DV1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="DV1" s="1" t="s">
+      <c r="DW1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="DW1" s="1" t="s">
+      <c r="DX1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="DX1" s="1" t="s">
+      <c r="DY1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="DY1" s="1" t="s">
+      <c r="DZ1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="DZ1" s="1" t="s">
+      <c r="EA1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="EA1" s="1" t="s">
+      <c r="EB1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="EB1" s="1" t="s">
+      <c r="EC1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="EC1" s="1" t="s">
+      <c r="ED1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="ED1" s="1" t="s">
+      <c r="EE1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="EE1" s="1" t="s">
+      <c r="EF1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="EF1" s="1" t="s">
+      <c r="EG1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="EG1" s="1" t="s">
+      <c r="EH1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="EH1" s="1" t="s">
+      <c r="EI1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="EI1" s="1" t="s">
+      <c r="EJ1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="EJ1" s="1" t="s">
+      <c r="EK1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="EK1" s="1" t="s">
+      <c r="EL1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="EL1" s="1" t="s">
+      <c r="EM1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="EM1" s="1" t="s">
+      <c r="EN1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="EN1" s="1" t="s">
+      <c r="EO1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="EO1" s="1" t="s">
+      <c r="EP1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="EP1" s="1" t="s">
+      <c r="EQ1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="EQ1" s="1" t="s">
+      <c r="ER1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="ER1" s="1" t="s">
+      <c r="ES1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="ES1" s="1" t="s">
+      <c r="ET1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="ET1" s="1" t="s">
+      <c r="EU1" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="EU1" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C2" s="2">
         <v>44000.592504050917</v>
@@ -2092,109 +2092,109 @@
         <v>44008</v>
       </c>
       <c r="E2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
       </c>
       <c r="G2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
         <v>161</v>
       </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
-        <v>162</v>
-      </c>
       <c r="K2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="N2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="O2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="P2" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q2" t="s">
         <v>199</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>200</v>
       </c>
       <c r="R2">
         <v>16055462485</v>
       </c>
       <c r="T2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="U2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="V2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="X2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AA2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AB2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AC2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AD2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AF2">
         <v>16055462485</v>
       </c>
       <c r="AI2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AJ2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AK2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AM2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AO2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="AP2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AQ2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AR2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AT2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AV2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AW2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AZ2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="BA2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="BB2" t="b">
         <v>0</v>
@@ -2215,10 +2215,10 @@
         <v>0</v>
       </c>
       <c r="BN2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="BO2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="BP2">
         <v>10</v>
@@ -2269,28 +2269,28 @@
         <v>8</v>
       </c>
       <c r="CF2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="CG2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="CH2">
         <v>14.99</v>
       </c>
       <c r="CI2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="CL2" t="b">
         <v>0</v>
       </c>
       <c r="CM2" t="s">
+        <v>313</v>
+      </c>
+      <c r="CO2" t="s">
         <v>314</v>
       </c>
-      <c r="CO2" t="s">
-        <v>315</v>
-      </c>
       <c r="CP2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="CQ2">
         <v>3</v>
@@ -2335,22 +2335,22 @@
         <v>0</v>
       </c>
       <c r="DF2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="DG2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="DH2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="DI2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="DJ2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="DK2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="DL2" t="b">
         <v>0</v>
@@ -2359,22 +2359,22 @@
         <v>1</v>
       </c>
       <c r="DN2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="DO2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="DP2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="DQ2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="DR2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="DS2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="DT2">
         <v>1</v>
@@ -2407,31 +2407,31 @@
         <v>55</v>
       </c>
       <c r="EE2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="EF2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="EH2">
         <v>0</v>
       </c>
       <c r="EI2" t="s">
+        <v>370</v>
+      </c>
+      <c r="EJ2" t="s">
         <v>371</v>
-      </c>
-      <c r="EJ2" t="s">
-        <v>372</v>
       </c>
       <c r="EK2" s="2">
         <v>44079.658868628961</v>
       </c>
       <c r="EL2" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="EM2" t="s">
+        <v>379</v>
+      </c>
+      <c r="EN2" t="s">
         <v>380</v>
-      </c>
-      <c r="EN2" t="s">
-        <v>381</v>
       </c>
       <c r="EO2">
         <v>1</v>
@@ -2443,7 +2443,7 @@
         <v>44.335346000000001</v>
       </c>
       <c r="ER2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="ES2">
         <v>1</v>
@@ -2457,10 +2457,10 @@
     </row>
     <row r="3" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C3" s="2">
         <v>43994.71920925926</v>
@@ -2469,112 +2469,112 @@
         <v>44012</v>
       </c>
       <c r="E3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H3" t="b">
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="O3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="R3">
         <v>12084594821</v>
       </c>
       <c r="T3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="U3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="V3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="X3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Y3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AA3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AB3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AC3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AD3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AF3">
         <v>12084594821</v>
       </c>
       <c r="AH3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AI3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AJ3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AK3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AL3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="AM3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AO3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AP3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AQ3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AR3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AT3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AV3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AW3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AZ3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="BA3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="BB3" t="b">
         <v>0</v>
@@ -2595,10 +2595,10 @@
         <v>0</v>
       </c>
       <c r="BN3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="BO3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="BP3">
         <v>19</v>
@@ -2649,28 +2649,28 @@
         <v>0</v>
       </c>
       <c r="CF3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="CG3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="CH3">
         <v>13.62</v>
       </c>
       <c r="CI3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="CL3" t="b">
         <v>1</v>
       </c>
       <c r="CM3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="CO3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="CP3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="CQ3">
         <v>3</v>
@@ -2715,22 +2715,22 @@
         <v>0</v>
       </c>
       <c r="DF3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="DG3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="DH3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="DI3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="DJ3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="DK3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="DL3" t="b">
         <v>1</v>
@@ -2739,22 +2739,22 @@
         <v>31</v>
       </c>
       <c r="DN3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="DO3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="DP3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="DQ3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="DR3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="DS3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="DT3">
         <v>1</v>
@@ -2790,31 +2790,31 @@
         <v>55</v>
       </c>
       <c r="EE3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="EF3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="EH3">
         <v>20</v>
       </c>
       <c r="EI3" t="s">
+        <v>370</v>
+      </c>
+      <c r="EJ3" t="s">
         <v>371</v>
-      </c>
-      <c r="EJ3" t="s">
-        <v>372</v>
       </c>
       <c r="EK3" s="2">
         <v>44079.658868628961</v>
       </c>
       <c r="EL3" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="EM3" t="s">
+        <v>379</v>
+      </c>
+      <c r="EN3" t="s">
         <v>380</v>
-      </c>
-      <c r="EN3" t="s">
-        <v>381</v>
       </c>
       <c r="EO3">
         <v>1</v>
@@ -2826,7 +2826,7 @@
         <v>43.575951000000003</v>
       </c>
       <c r="ER3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="ES3">
         <v>1</v>
@@ -2840,10 +2840,10 @@
     </row>
     <row r="4" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C4" s="2">
         <v>43992.692545601851</v>
@@ -2852,121 +2852,121 @@
         <v>44007</v>
       </c>
       <c r="E4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="O4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="P4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="R4">
         <v>12794344124</v>
       </c>
       <c r="T4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="U4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="V4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="X4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="Y4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AA4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AB4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AC4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AD4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AF4">
         <v>12704344124</v>
       </c>
       <c r="AH4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AI4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AJ4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AK4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AL4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AM4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AO4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AP4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AQ4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AR4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AT4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AV4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AW4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="AX4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AY4" t="s">
+        <v>283</v>
+      </c>
+      <c r="AZ4" t="s">
         <v>284</v>
       </c>
-      <c r="AZ4" t="s">
-        <v>285</v>
-      </c>
       <c r="BA4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="BB4" t="b">
         <v>0</v>
@@ -2987,10 +2987,10 @@
         <v>0</v>
       </c>
       <c r="BN4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="BO4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="BP4">
         <v>1</v>
@@ -3038,16 +3038,16 @@
         <v>5</v>
       </c>
       <c r="CF4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="CG4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="CH4">
         <v>17.5</v>
       </c>
       <c r="CI4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="CJ4">
         <v>0</v>
@@ -3056,13 +3056,13 @@
         <v>0</v>
       </c>
       <c r="CM4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="CO4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="CP4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="CQ4">
         <v>3</v>
@@ -3107,22 +3107,22 @@
         <v>0</v>
       </c>
       <c r="DF4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="DG4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="DH4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="DI4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="DJ4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="DK4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="DL4" t="b">
         <v>0</v>
@@ -3131,22 +3131,22 @@
         <v>1</v>
       </c>
       <c r="DN4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="DO4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="DP4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="DQ4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="DR4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="DS4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="DT4">
         <v>1</v>
@@ -3179,34 +3179,34 @@
         <v>55</v>
       </c>
       <c r="EE4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="EF4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="EG4" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="EH4">
         <v>0</v>
       </c>
       <c r="EI4" t="s">
+        <v>370</v>
+      </c>
+      <c r="EJ4" t="s">
         <v>371</v>
-      </c>
-      <c r="EJ4" t="s">
-        <v>372</v>
       </c>
       <c r="EK4" s="2">
         <v>44079.658868628961</v>
       </c>
       <c r="EL4" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="EM4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="EN4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="EO4">
         <v>1</v>
@@ -3218,7 +3218,7 @@
         <v>36.808073</v>
       </c>
       <c r="ER4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="ES4">
         <v>1</v>
@@ -3232,10 +3232,10 @@
     </row>
     <row r="5" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C5" s="2">
         <v>43992.621228587966</v>
@@ -3244,112 +3244,112 @@
         <v>44012</v>
       </c>
       <c r="E5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
         <v>160</v>
       </c>
-      <c r="F5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
-        <v>161</v>
-      </c>
       <c r="H5" t="b">
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="N5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="P5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="R5">
         <v>15093935775</v>
       </c>
       <c r="T5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="U5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="V5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="X5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Y5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AA5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AB5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AC5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AD5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AF5">
         <v>15093935775</v>
       </c>
       <c r="AH5" t="s">
+        <v>230</v>
+      </c>
+      <c r="AI5" t="s">
         <v>231</v>
       </c>
-      <c r="AI5" t="s">
-        <v>232</v>
-      </c>
       <c r="AJ5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AK5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AM5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AN5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AO5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AP5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AQ5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="AR5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AT5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AV5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="AW5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AZ5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="BA5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="BB5" t="b">
         <v>0</v>
@@ -3370,10 +3370,10 @@
         <v>1</v>
       </c>
       <c r="BN5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="BO5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="BP5">
         <v>14</v>
@@ -3424,34 +3424,34 @@
         <v>5</v>
       </c>
       <c r="CF5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="CG5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="CH5">
         <v>15.83</v>
       </c>
       <c r="CI5" t="s">
+        <v>311</v>
+      </c>
+      <c r="CJ5">
+        <v>0</v>
+      </c>
+      <c r="CK5" t="s">
         <v>312</v>
       </c>
-      <c r="CJ5">
-        <v>0</v>
-      </c>
-      <c r="CK5" t="s">
+      <c r="CL5" t="b">
+        <v>0</v>
+      </c>
+      <c r="CM5" t="s">
         <v>313</v>
       </c>
-      <c r="CL5" t="b">
-        <v>0</v>
-      </c>
-      <c r="CM5" t="s">
-        <v>314</v>
-      </c>
       <c r="CO5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="CP5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="CQ5">
         <v>3</v>
@@ -3496,22 +3496,22 @@
         <v>0</v>
       </c>
       <c r="DF5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="DG5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="DH5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="DI5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="DJ5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="DK5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="DL5" t="b">
         <v>1</v>
@@ -3520,22 +3520,22 @@
         <v>4</v>
       </c>
       <c r="DN5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="DO5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="DP5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="DQ5" t="s">
+        <v>347</v>
+      </c>
+      <c r="DR5" t="s">
         <v>348</v>
       </c>
-      <c r="DR5" t="s">
-        <v>349</v>
-      </c>
       <c r="DS5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="DT5">
         <v>41</v>
@@ -3571,34 +3571,34 @@
         <v>55</v>
       </c>
       <c r="EE5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="EF5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="EG5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="EH5">
         <v>0</v>
       </c>
       <c r="EI5" t="s">
+        <v>370</v>
+      </c>
+      <c r="EJ5" t="s">
         <v>371</v>
-      </c>
-      <c r="EJ5" t="s">
-        <v>372</v>
       </c>
       <c r="EK5" s="2">
         <v>44079.658868628961</v>
       </c>
       <c r="EL5" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="EM5" t="s">
+        <v>379</v>
+      </c>
+      <c r="EN5" t="s">
         <v>380</v>
-      </c>
-      <c r="EN5" t="s">
-        <v>381</v>
       </c>
       <c r="EO5">
         <v>1</v>
@@ -3610,7 +3610,7 @@
         <v>47.741219000000001</v>
       </c>
       <c r="ER5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="ES5">
         <v>1</v>
@@ -3624,10 +3624,10 @@
     </row>
     <row r="6" spans="1:151" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C6" s="2">
         <v>43992.569384027767</v>
@@ -3636,121 +3636,121 @@
         <v>44012</v>
       </c>
       <c r="E6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="R6">
         <v>15152959666</v>
       </c>
       <c r="T6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="U6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="V6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="W6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="X6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="Y6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="Z6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AA6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AB6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AC6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AD6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AF6">
         <v>15152959666</v>
       </c>
       <c r="AI6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AJ6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AK6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AL6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AM6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AN6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AO6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AP6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AQ6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AR6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AT6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="AV6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AW6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AZ6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="BA6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="BB6" t="b">
         <v>1</v>
@@ -3771,10 +3771,10 @@
         <v>0</v>
       </c>
       <c r="BN6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="BO6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="BP6">
         <v>2</v>
@@ -3825,28 +3825,28 @@
         <v>0</v>
       </c>
       <c r="CF6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="CG6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="CH6">
         <v>14.58</v>
       </c>
       <c r="CI6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="CL6" t="b">
         <v>1</v>
       </c>
       <c r="CM6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="CO6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="CP6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="CQ6">
         <v>3</v>
@@ -3891,22 +3891,22 @@
         <v>0</v>
       </c>
       <c r="DF6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="DG6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="DH6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="DI6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="DJ6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="DK6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="DL6" t="b">
         <v>1</v>
@@ -3915,22 +3915,22 @@
         <v>8</v>
       </c>
       <c r="DN6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="DO6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="DP6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="DQ6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="DR6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="DS6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="DT6">
         <v>1</v>
@@ -3963,34 +3963,34 @@
         <v>55</v>
       </c>
       <c r="EE6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="EF6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="EG6" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="EH6">
         <v>2</v>
       </c>
       <c r="EI6" t="s">
+        <v>370</v>
+      </c>
+      <c r="EJ6" t="s">
         <v>371</v>
-      </c>
-      <c r="EJ6" t="s">
-        <v>372</v>
       </c>
       <c r="EK6" s="2">
         <v>44079.658868628961</v>
       </c>
       <c r="EL6" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="EM6" t="s">
+        <v>379</v>
+      </c>
+      <c r="EN6" t="s">
         <v>380</v>
-      </c>
-      <c r="EN6" t="s">
-        <v>381</v>
       </c>
       <c r="EO6">
         <v>1</v>
@@ -4002,7 +4002,7 @@
         <v>43.082701999999998</v>
       </c>
       <c r="ER6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="ES6">
         <v>1</v>
@@ -4016,10 +4016,10 @@
     </row>
     <row r="7" spans="1:151" ht="86" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C7" s="2">
         <v>43992.418642708333</v>
@@ -4028,115 +4028,115 @@
         <v>44012</v>
       </c>
       <c r="E7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="R7">
         <v>12187836610</v>
       </c>
       <c r="T7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="U7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="V7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="W7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="X7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="Y7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AA7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AB7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AC7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AD7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AF7">
         <v>12187836610</v>
       </c>
       <c r="AI7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AJ7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AK7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AL7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AM7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AN7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AO7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AP7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AQ7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AR7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AT7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="AV7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AW7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AZ7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="BA7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="BB7" t="b">
         <v>0</v>
@@ -4157,10 +4157,10 @@
         <v>0</v>
       </c>
       <c r="BN7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="BO7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="BP7">
         <v>5</v>
@@ -4211,28 +4211,28 @@
         <v>8</v>
       </c>
       <c r="CF7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="CG7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="CH7">
         <v>14.4</v>
       </c>
       <c r="CI7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="CL7" t="b">
         <v>1</v>
       </c>
       <c r="CM7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="CO7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="CP7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="CQ7">
         <v>3</v>
@@ -4274,22 +4274,22 @@
         <v>0</v>
       </c>
       <c r="DF7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="DG7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="DH7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="DI7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="DJ7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="DK7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="DL7" t="b">
         <v>0</v>
@@ -4298,22 +4298,22 @@
         <v>1</v>
       </c>
       <c r="DN7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="DO7" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="DP7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="DQ7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="DR7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="DS7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="DT7">
         <v>2</v>
@@ -4346,34 +4346,34 @@
         <v>55</v>
       </c>
       <c r="EE7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="EF7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="EG7" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="EH7">
+        <v>1</v>
+      </c>
+      <c r="EI7" t="s">
         <v>370</v>
       </c>
-      <c r="EH7">
-        <v>1</v>
-      </c>
-      <c r="EI7" t="s">
+      <c r="EJ7" t="s">
         <v>371</v>
-      </c>
-      <c r="EJ7" t="s">
-        <v>372</v>
       </c>
       <c r="EK7" s="2">
         <v>44079.658868628961</v>
       </c>
       <c r="EL7" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="EM7" t="s">
+        <v>379</v>
+      </c>
+      <c r="EN7" t="s">
         <v>380</v>
-      </c>
-      <c r="EN7" t="s">
-        <v>381</v>
       </c>
       <c r="EO7">
         <v>1</v>
@@ -4385,7 +4385,7 @@
         <v>48.866801000000002</v>
       </c>
       <c r="ER7" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="ES7">
         <v>1</v>
@@ -4399,10 +4399,10 @@
     </row>
     <row r="8" spans="1:151" ht="71" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" t="s">
         <v>156</v>
-      </c>
-      <c r="B8" t="s">
-        <v>157</v>
       </c>
       <c r="C8" s="2">
         <v>43992.355112962963</v>
@@ -4411,121 +4411,121 @@
         <v>44012</v>
       </c>
       <c r="E8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="N8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O8" t="s">
+        <v>197</v>
+      </c>
+      <c r="P8" t="s">
         <v>198</v>
-      </c>
-      <c r="P8" t="s">
-        <v>199</v>
       </c>
       <c r="R8">
         <v>16419852502</v>
       </c>
       <c r="T8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="U8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="V8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W8" t="s">
+        <v>221</v>
+      </c>
+      <c r="X8" t="s">
         <v>222</v>
       </c>
-      <c r="X8" t="s">
-        <v>223</v>
-      </c>
       <c r="Y8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Z8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AA8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AB8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AC8" t="s">
+        <v>197</v>
+      </c>
+      <c r="AD8" t="s">
         <v>198</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>199</v>
       </c>
       <c r="AF8">
         <v>16419852502</v>
       </c>
       <c r="AI8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AJ8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AK8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AL8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AM8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AN8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AO8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AP8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AQ8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AR8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AT8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="AV8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AW8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AZ8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="BA8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="BB8" t="b">
         <v>0</v>
@@ -4546,10 +4546,10 @@
         <v>0</v>
       </c>
       <c r="BN8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="BO8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="BP8">
         <v>2</v>
@@ -4600,28 +4600,28 @@
         <v>5</v>
       </c>
       <c r="CF8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="CG8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="CH8">
         <v>14.58</v>
       </c>
       <c r="CI8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="CL8" t="b">
         <v>1</v>
       </c>
       <c r="CM8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="CO8" t="s">
+        <v>319</v>
+      </c>
+      <c r="CP8" t="s">
         <v>320</v>
-      </c>
-      <c r="CP8" t="s">
-        <v>321</v>
       </c>
       <c r="CQ8">
         <v>3</v>
@@ -4663,22 +4663,22 @@
         <v>0</v>
       </c>
       <c r="DF8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="DG8" t="s">
+        <v>329</v>
+      </c>
+      <c r="DH8" t="s">
         <v>330</v>
       </c>
-      <c r="DH8" t="s">
+      <c r="DI8" t="s">
+        <v>189</v>
+      </c>
+      <c r="DJ8" t="s">
         <v>331</v>
       </c>
-      <c r="DI8" t="s">
-        <v>190</v>
-      </c>
-      <c r="DJ8" t="s">
-        <v>332</v>
-      </c>
       <c r="DK8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="DL8" t="b">
         <v>0</v>
@@ -4687,22 +4687,22 @@
         <v>1</v>
       </c>
       <c r="DN8" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="DO8" t="s">
+        <v>330</v>
+      </c>
+      <c r="DP8" t="s">
+        <v>189</v>
+      </c>
+      <c r="DQ8" t="s">
         <v>331</v>
       </c>
-      <c r="DP8" t="s">
-        <v>190</v>
-      </c>
-      <c r="DQ8" t="s">
-        <v>332</v>
-      </c>
       <c r="DR8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="DS8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="DT8">
         <v>1</v>
@@ -4735,34 +4735,34 @@
         <v>55</v>
       </c>
       <c r="EE8" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="EF8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="EG8" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="EH8">
         <v>1</v>
       </c>
       <c r="EI8" t="s">
+        <v>370</v>
+      </c>
+      <c r="EJ8" t="s">
         <v>371</v>
-      </c>
-      <c r="EJ8" t="s">
-        <v>372</v>
       </c>
       <c r="EK8" s="2">
         <v>44079.658868628961</v>
       </c>
       <c r="EL8" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="EM8" t="s">
         <v>379</v>
       </c>
-      <c r="EM8" t="s">
+      <c r="EN8" t="s">
         <v>380</v>
-      </c>
-      <c r="EN8" t="s">
-        <v>381</v>
       </c>
       <c r="EO8">
         <v>1</v>
@@ -4774,7 +4774,7 @@
         <v>43.400039999999997</v>
       </c>
       <c r="ER8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="ES8">
         <v>1</v>

</xml_diff>

<commit_message>
adds scripts to add extra quarterly dol files
</commit_message>
<xml_diff>
--- a/excel_files/accurate_dol_geocoded.xlsx
+++ b/excel_files/accurate_dol_geocoded.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexpiazza/Desktop/for_db/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FEAFC36-E29E-9E4C-B2C0-B2E1C4D92057}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4965FB35-2531-104F-9DAD-CBCBDEDBD3C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="384">
   <si>
     <t>CASE_NUMBER</t>
   </si>
@@ -1605,8 +1605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:EU8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BZ1" workbookViewId="0">
-      <selection activeCell="CN1" sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="CY1" workbookViewId="0">
+      <selection activeCell="DJ7" sqref="DJ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1615,7 +1615,9 @@
     <col min="7" max="7" width="20.5" customWidth="1"/>
     <col min="9" max="9" width="36.1640625" customWidth="1"/>
     <col min="10" max="10" width="34.5" customWidth="1"/>
+    <col min="67" max="67" width="18" customWidth="1"/>
     <col min="112" max="112" width="29.1640625" customWidth="1"/>
+    <col min="114" max="114" width="25.5" customWidth="1"/>
     <col min="118" max="118" width="29.33203125" customWidth="1"/>
     <col min="119" max="119" width="23.6640625" customWidth="1"/>
     <col min="144" max="144" width="33.83203125" customWidth="1"/>
@@ -4284,9 +4286,6 @@
       </c>
       <c r="DI7" t="s">
         <v>190</v>
-      </c>
-      <c r="DJ7" t="s">
-        <v>196</v>
       </c>
       <c r="DK7" t="s">
         <v>337</v>

</xml_diff>